<commit_message>
update template yeu cau mua hang
</commit_message>
<xml_diff>
--- a/addons/custom/purchase_request/static/src/xlsx/template_import_pr.xlsx
+++ b/addons/custom/purchase_request/static/src/xlsx/template_import_pr.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Project\m_onnet_odoo_mfl2201er\addons\custom\purchase_request\static\src\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FORLIFE\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039388E1-41A5-4B68-BFE8-4C9A6C6CEFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C989DF7-6363-48C6-8E87-4B6109DAC4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Yêu cầu mua hàng" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Mã vụ việc</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>1521_NPL</t>
-  </si>
-  <si>
-    <t>Đơn vị</t>
   </si>
   <si>
     <r>
@@ -100,20 +97,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (*)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Chi tiết đơn hàng / Đơn vị mua </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(*)</t>
     </r>
   </si>
   <si>
@@ -591,33 +574,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="30.88671875" customWidth="1"/>
-    <col min="9" max="9" width="36.44140625" customWidth="1"/>
-    <col min="10" max="10" width="33.6640625" customWidth="1"/>
-    <col min="11" max="11" width="31.109375" customWidth="1"/>
-    <col min="12" max="12" width="30.88671875" style="7" customWidth="1"/>
-    <col min="13" max="13" width="32" customWidth="1"/>
-    <col min="14" max="14" width="35.5546875" customWidth="1"/>
-    <col min="15" max="15" width="32.6640625" style="11" customWidth="1"/>
-    <col min="16" max="16" width="39.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" customWidth="1"/>
+    <col min="10" max="10" width="33.7109375" customWidth="1"/>
+    <col min="11" max="11" width="30.85546875" style="7" customWidth="1"/>
+    <col min="12" max="12" width="32" customWidth="1"/>
+    <col min="13" max="13" width="35.5703125" customWidth="1"/>
+    <col min="14" max="14" width="32.7109375" style="11" customWidth="1"/>
+    <col min="15" max="15" width="39.140625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -628,13 +610,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -643,31 +625,28 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="M1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="N1" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="O1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1405000168</v>
       </c>
@@ -692,17 +671,14 @@
       <c r="J2">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
-        <v>10</v>
+      <c r="N2" s="9">
+        <v>45122</v>
       </c>
       <c r="O2" s="9">
         <v>45122</v>
       </c>
-      <c r="P2" s="9">
-        <v>45122</v>
-      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
     </row>
   </sheetData>

</xml_diff>